<commit_message>
fix: only place comment about column only in location if no value.
</commit_message>
<xml_diff>
--- a/Compare_excel_library/assets/comparison.xlsx
+++ b/Compare_excel_library/assets/comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\excel-comparer\Compare_excel_library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\excel-comparer\Compare_excel_library\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68154CD9-D3D1-49DD-BEBD-7BC1FC19CDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80104ABE-D831-4E07-9CD2-53EED4BE2379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{B4B7EED7-061B-4FA7-BF35-A8BC32693F8A}"/>
+    <workbookView xWindow="8340" yWindow="1524" windowWidth="13800" windowHeight="7092" xr2:uid="{B4B7EED7-061B-4FA7-BF35-A8BC32693F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.23</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>

</xml_diff>